<commit_message>
implemented new equations, updated input, and have first running version
</commit_message>
<xml_diff>
--- a/Test_Input_Paired.xlsx
+++ b/Test_Input_Paired.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20379"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9280E94A-6272-4FC6-80CE-17A582F44163}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CD535C-8BAE-444D-93DC-3C1AD22329E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10Be Cronus" sheetId="3" r:id="rId1"/>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="13">
-        <v>42920</v>
+        <v>63299</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="13">
-        <v>273141</v>
+        <v>216620</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1903,7 +1903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B805AF-634F-468E-AD2E-541576FB2895}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adjusted test data to match 100mm/ka again
</commit_message>
<xml_diff>
--- a/Test_Input_Paired.xlsx
+++ b/Test_Input_Paired.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20380"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CD535C-8BAE-444D-93DC-3C1AD22329E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE752912-9168-4904-8B65-D1616AA7D7B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10Be Cronus" sheetId="3" r:id="rId1"/>
@@ -867,38 +867,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3984375" customWidth="1"/>
-    <col min="9" max="9" width="11.86328125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.3984375" customWidth="1"/>
-    <col min="15" max="15" width="22.59765625" customWidth="1"/>
-    <col min="16" max="16" width="15.1328125" customWidth="1"/>
-    <col min="17" max="17" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.3984375" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -999,7 +999,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>90</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="13">
-        <v>63299</v>
+        <v>64188</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -1143,13 +1143,13 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="15" t="s">
         <v>105</v>
@@ -1196,42 +1196,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CB7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="11.3984375" customWidth="1"/>
-    <col min="12" max="12" width="16.1328125" customWidth="1"/>
-    <col min="13" max="13" width="21.3984375" customWidth="1"/>
-    <col min="14" max="14" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.86328125" customWidth="1"/>
-    <col min="19" max="35" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="35" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="25" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="13">
-        <v>216620</v>
+        <v>216885</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1882,13 +1882,13 @@
       <c r="BZ3" s="8"/>
       <c r="CA3" s="8"/>
     </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="15" t="s">
         <v>105</v>
@@ -1907,15 +1907,15 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -1973,13 +1973,13 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="15" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
imporved commenting and documentation; removed bug from attenuation length basin calculation by making sure the DEM is cropped to the basin before calculation
</commit_message>
<xml_diff>
--- a/Test_Input_Paired.xlsx
+++ b/Test_Input_Paired.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20380"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE752912-9168-4904-8B65-D1616AA7D7B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="10Be Cronus" sheetId="3" r:id="rId1"/>
     <sheet name="36Cl Cronus" sheetId="5" r:id="rId2"/>
     <sheet name="Composition and other" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="125">
   <si>
     <t>Sample</t>
   </si>
@@ -382,23 +381,26 @@
     <t>scaling model (st,sf,sa…)</t>
   </si>
   <si>
-    <t>soil mass (g/cm2)</t>
-  </si>
-  <si>
     <t>st</t>
   </si>
   <si>
     <t>requires either bedrock or soil composition</t>
+  </si>
+  <si>
+    <t>required input (can mostly be replaced by zeros if not measured)</t>
+  </si>
+  <si>
+    <t>regolith mass (g/cm2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,6 +425,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -501,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -509,14 +517,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -527,6 +530,16 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,23 +633,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -672,23 +668,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -864,41 +843,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="15" max="15" width="22.5546875" customWidth="1"/>
+    <col min="16" max="16" width="15.109375" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.42578125" customWidth="1"/>
+    <col min="32" max="32" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -999,7 +978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
@@ -1102,32 +1081,32 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="8">
         <v>48.585000000000001</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>9.25</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="14">
         <v>345</v>
       </c>
       <c r="F3">
         <v>6.25E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="23">
         <v>2.6</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="23">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="23">
         <v>0</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="10">
         <v>64188</v>
       </c>
       <c r="O3">
@@ -1139,19 +1118,19 @@
       <c r="V3">
         <v>0.1</v>
       </c>
-      <c r="Y3" s="13">
+      <c r="Y3" s="10">
         <v>4300</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="15" t="s">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="12" t="s">
         <v>105</v>
       </c>
       <c r="C7" s="4"/>
@@ -1193,45 +1172,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AW3" sqref="AW3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" customWidth="1"/>
-    <col min="19" max="35" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.88671875" customWidth="1"/>
+    <col min="19" max="35" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="25" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1473,7 +1452,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:80" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1712,32 +1691,32 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:80" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="8">
         <v>48.585000000000001</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>9.25</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="14">
         <v>345</v>
       </c>
       <c r="F3">
         <v>6.25E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="8">
         <v>2.6</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="8">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="8">
         <v>0</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="10">
         <v>216885</v>
       </c>
       <c r="M3">
@@ -1749,148 +1728,148 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="8">
         <v>15.11</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="8">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="8">
         <v>1.3</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="8">
         <v>1.37</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="8">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="8">
         <v>0.45</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="8">
         <v>44.79</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="8">
         <v>0.11</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="8">
         <v>0.26</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="8">
         <v>0.08</v>
       </c>
-      <c r="Z3" s="7">
+      <c r="Z3" s="18">
         <v>0</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="8">
         <v>37.06</v>
       </c>
-      <c r="AB3" s="9">
+      <c r="AB3" s="19">
         <v>26.94</v>
       </c>
-      <c r="AC3" s="7">
+      <c r="AC3" s="18">
         <v>0</v>
       </c>
-      <c r="AD3" s="10">
+      <c r="AD3" s="20">
         <v>2.7</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="8">
         <v>2.4</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="8">
         <v>0.8</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="8">
         <v>2.5</v>
       </c>
-      <c r="AH3" s="8">
+      <c r="AH3" s="21">
         <v>0</v>
       </c>
-      <c r="AI3" s="8">
+      <c r="AI3" s="21">
         <v>0</v>
       </c>
-      <c r="AJ3">
+      <c r="AJ3" s="8">
         <v>0</v>
       </c>
-      <c r="AK3">
+      <c r="AK3" s="8">
         <v>56.757492528031307</v>
       </c>
-      <c r="AL3">
+      <c r="AL3" s="8">
         <v>1.0574911744800741E-2</v>
       </c>
-      <c r="AM3">
+      <c r="AM3" s="8">
         <v>0.8971040222421397</v>
       </c>
-      <c r="AN3" s="9">
+      <c r="AN3" s="19">
         <v>26.94</v>
       </c>
-      <c r="AO3" s="8">
+      <c r="AO3" s="7">
         <v>0</v>
       </c>
-      <c r="AP3" s="8">
+      <c r="AP3" s="7">
         <v>0</v>
       </c>
-      <c r="AQ3" s="8">
+      <c r="AQ3" s="7">
         <v>0</v>
       </c>
-      <c r="AR3" s="8">
+      <c r="AR3" s="7">
         <v>0</v>
       </c>
-      <c r="AS3" s="8">
+      <c r="AS3" s="7">
         <v>0</v>
       </c>
       <c r="AT3">
         <v>0.1</v>
       </c>
-      <c r="AU3" s="8">
+      <c r="AU3" s="7">
         <v>0</v>
       </c>
-      <c r="AV3" s="8">
+      <c r="AV3" s="7">
         <v>0</v>
       </c>
-      <c r="AW3" s="13">
+      <c r="AW3" s="22">
         <v>12100</v>
       </c>
-      <c r="AX3" s="8"/>
-      <c r="AY3" s="8"/>
-      <c r="AZ3" s="8"/>
-      <c r="BA3" s="8"/>
-      <c r="BB3" s="8"/>
-      <c r="BC3" s="8"/>
-      <c r="BD3" s="8"/>
-      <c r="BE3" s="8"/>
-      <c r="BF3" s="8"/>
-      <c r="BG3" s="8"/>
-      <c r="BH3" s="8"/>
-      <c r="BI3" s="8"/>
-      <c r="BJ3" s="8"/>
-      <c r="BK3" s="8"/>
-      <c r="BL3" s="8"/>
-      <c r="BM3" s="8"/>
-      <c r="BN3" s="8"/>
-      <c r="BO3" s="8"/>
-      <c r="BP3" s="8"/>
-      <c r="BQ3" s="8"/>
-      <c r="BR3" s="8"/>
-      <c r="BS3" s="8"/>
-      <c r="BT3" s="8"/>
-      <c r="BU3" s="8"/>
-      <c r="BV3" s="8"/>
-      <c r="BW3" s="8"/>
-      <c r="BX3" s="8"/>
-      <c r="BY3" s="8"/>
-      <c r="BZ3" s="8"/>
-      <c r="CA3" s="8"/>
+      <c r="AX3" s="7"/>
+      <c r="AY3" s="7"/>
+      <c r="AZ3" s="7"/>
+      <c r="BA3" s="7"/>
+      <c r="BB3" s="7"/>
+      <c r="BC3" s="7"/>
+      <c r="BD3" s="7"/>
+      <c r="BE3" s="7"/>
+      <c r="BF3" s="7"/>
+      <c r="BG3" s="7"/>
+      <c r="BH3" s="7"/>
+      <c r="BI3" s="7"/>
+      <c r="BJ3" s="7"/>
+      <c r="BK3" s="7"/>
+      <c r="BL3" s="7"/>
+      <c r="BM3" s="7"/>
+      <c r="BN3" s="7"/>
+      <c r="BO3" s="7"/>
+      <c r="BP3" s="7"/>
+      <c r="BQ3" s="7"/>
+      <c r="BR3" s="7"/>
+      <c r="BS3" s="7"/>
+      <c r="BT3" s="7"/>
+      <c r="BU3" s="7"/>
+      <c r="BV3" s="7"/>
+      <c r="BW3" s="7"/>
+      <c r="BX3" s="7"/>
+      <c r="BY3" s="7"/>
+      <c r="BZ3" s="7"/>
+      <c r="CA3" s="7"/>
     </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+    <row r="6" spans="1:80" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="15" t="s">
+    <row r="7" spans="1:80" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="12" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1900,22 +1879,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B805AF-634F-468E-AD2E-541576FB2895}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1937,52 +1916,52 @@
       <c r="G1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="14">
         <v>0.05</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="14">
         <v>0.7</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="14">
         <v>0.25</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16">
         <v>200</v>
       </c>
-      <c r="I2" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="J2" s="19" t="s">
+      <c r="I2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="15" t="s">
-        <v>123</v>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="12" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated README, updated input concentrations in example for decay
</commit_message>
<xml_diff>
--- a/Test_Input_Paired.xlsx
+++ b/Test_Input_Paired.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20385"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638C5D96-ACDE-40ED-8977-38ACBF49C733}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10Be Cronus" sheetId="3" r:id="rId1"/>
@@ -396,7 +397,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -633,6 +634,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -668,6 +686,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -843,41 +878,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
-    <col min="15" max="15" width="22.5546875" customWidth="1"/>
-    <col min="16" max="16" width="15.109375" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.44140625" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -978,7 +1013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
@@ -1081,7 +1116,7 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>90</v>
       </c>
@@ -1107,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="10">
-        <v>64188</v>
+        <v>63814</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -1122,13 +1157,13 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="12" t="s">
         <v>105</v>
@@ -1172,45 +1207,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CB7"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AW3" sqref="AW3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1"/>
-    <col min="13" max="13" width="21.44140625" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.88671875" customWidth="1"/>
-    <col min="19" max="35" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="35" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="25" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1452,7 +1487,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1691,7 +1726,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -1717,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="10">
-        <v>216885</v>
+        <v>215142</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -1861,13 +1896,13 @@
       <c r="BZ3" s="7"/>
       <c r="CA3" s="7"/>
     </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="12" t="s">
         <v>105</v>
@@ -1879,22 +1914,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +1961,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -1952,13 +1987,13 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="12" t="s">
         <v>122</v>

</xml_diff>